<commit_message>
v2.0: Ranking dinamico por grupos SISBEN y nuevo shapefile
Cambios principales:
- Nuevo shapefile de UPZ (Datos Abiertos Bogota 2022)
- Ranking dinamico: selecciona grupos A, B, C, D para recalcular
- Tab de comparacion de rankings (original vs dinamico)
- Correccion de duplicados en datos (LA FLORA, PARQUE ENTRENUBES)
- Mapa con geometrias completas de 112 UPZ
- Actualizacion de dependencias (geopandas)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Tabla_Completa_Priorizacion_JCO.xlsx
+++ b/Tabla_Completa_Priorizacion_JCO.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="148">
   <si>
     <t>RANKING</t>
   </si>
@@ -815,7 +815,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R115"/>
+  <dimension ref="A1:R113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6311,140 +6311,140 @@
     </row>
     <row r="99" spans="1:18">
       <c r="A99">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B99">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="C99" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="D99" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E99">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F99">
         <v>78</v>
       </c>
       <c r="G99">
+        <v>6</v>
+      </c>
+      <c r="H99">
+        <v>31</v>
+      </c>
+      <c r="I99">
+        <v>34</v>
+      </c>
+      <c r="J99">
+        <v>7</v>
+      </c>
+      <c r="K99">
+        <v>3</v>
+      </c>
+      <c r="L99">
         <v>21</v>
       </c>
-      <c r="H99">
-        <v>27</v>
-      </c>
-      <c r="I99">
-        <v>27</v>
-      </c>
-      <c r="J99">
+      <c r="M99">
+        <v>18</v>
+      </c>
+      <c r="N99">
         <v>3</v>
       </c>
-      <c r="K99">
-        <v>11</v>
-      </c>
-      <c r="L99">
-        <v>14</v>
-      </c>
-      <c r="M99">
-        <v>15</v>
-      </c>
-      <c r="N99">
-        <v>2</v>
-      </c>
       <c r="O99">
+        <v>3</v>
+      </c>
+      <c r="P99">
         <v>10</v>
       </c>
-      <c r="P99">
-        <v>13</v>
-      </c>
       <c r="Q99">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R99">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:18">
       <c r="A100">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B100">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C100" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D100" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E100">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="F100">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="G100">
+        <v>3</v>
+      </c>
+      <c r="H100">
+        <v>18</v>
+      </c>
+      <c r="I100">
+        <v>28</v>
+      </c>
+      <c r="J100">
+        <v>3</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
         <v>6</v>
       </c>
-      <c r="H100">
-        <v>31</v>
-      </c>
-      <c r="I100">
-        <v>34</v>
-      </c>
-      <c r="J100">
-        <v>7</v>
-      </c>
-      <c r="K100">
-        <v>3</v>
-      </c>
-      <c r="L100">
-        <v>21</v>
-      </c>
       <c r="M100">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="N100">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O100">
         <v>3</v>
       </c>
       <c r="P100">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q100">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R100">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:18">
       <c r="A101">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B101">
+        <v>103</v>
+      </c>
+      <c r="C101" t="s">
         <v>117</v>
       </c>
-      <c r="C101" t="s">
-        <v>116</v>
-      </c>
       <c r="D101" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E101">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F101">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G101">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H101">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I101">
         <v>28</v>
@@ -6453,116 +6453,116 @@
         <v>3</v>
       </c>
       <c r="K101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L101">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M101">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="N101">
+        <v>2</v>
+      </c>
+      <c r="O101">
+        <v>0</v>
+      </c>
+      <c r="P101">
+        <v>7</v>
+      </c>
+      <c r="Q101">
+        <v>14</v>
+      </c>
+      <c r="R101">
         <v>1</v>
-      </c>
-      <c r="O101">
-        <v>3</v>
-      </c>
-      <c r="P101">
-        <v>12</v>
-      </c>
-      <c r="Q101">
-        <v>17</v>
-      </c>
-      <c r="R101">
-        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:18">
       <c r="A102">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B102">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C102" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D102" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E102">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F102">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="G102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H102">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I102">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="J102">
+        <v>44</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
         <v>3</v>
       </c>
-      <c r="K102">
-        <v>1</v>
-      </c>
-      <c r="L102">
-        <v>7</v>
-      </c>
       <c r="M102">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="N102">
+        <v>24</v>
+      </c>
+      <c r="O102">
+        <v>0</v>
+      </c>
+      <c r="P102">
         <v>2</v>
       </c>
-      <c r="O102">
-        <v>0</v>
-      </c>
-      <c r="P102">
-        <v>7</v>
-      </c>
       <c r="Q102">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="R102">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:18">
       <c r="A103">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B103">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C103" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D103" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E103">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F103">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H103">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I103">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J103">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="K103">
         <v>0</v>
@@ -6571,54 +6571,54 @@
         <v>3</v>
       </c>
       <c r="M103">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N103">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O103">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q103">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="R103">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:18">
       <c r="A104">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B104">
-        <v>106</v>
+        <v>20</v>
       </c>
       <c r="C104" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D104" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="E104">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="F104">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="G104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H104">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I104">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="J104">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="K104">
         <v>0</v>
@@ -6627,243 +6627,243 @@
         <v>3</v>
       </c>
       <c r="M104">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="N104">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="O104">
+        <v>0</v>
+      </c>
+      <c r="P104">
         <v>2</v>
       </c>
-      <c r="P104">
-        <v>1</v>
-      </c>
       <c r="Q104">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="R104">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:18">
       <c r="A105">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B105">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="C105" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D105" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="E105">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F105">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="G105">
         <v>0</v>
       </c>
       <c r="H105">
+        <v>6</v>
+      </c>
+      <c r="I105">
+        <v>10</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105">
         <v>5</v>
       </c>
-      <c r="I105">
-        <v>16</v>
-      </c>
-      <c r="J105">
-        <v>6</v>
-      </c>
-      <c r="K105">
-        <v>0</v>
-      </c>
-      <c r="L105">
-        <v>3</v>
-      </c>
       <c r="M105">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N105">
+        <v>0</v>
+      </c>
+      <c r="O105">
+        <v>0</v>
+      </c>
+      <c r="P105">
         <v>1</v>
       </c>
-      <c r="O105">
-        <v>0</v>
-      </c>
-      <c r="P105">
-        <v>2</v>
-      </c>
       <c r="Q105">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="R105">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:18">
       <c r="A106">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B106">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="C106" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D106" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E106">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F106">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H106">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I106">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K106">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L106">
+        <v>2</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="N106">
+        <v>0</v>
+      </c>
+      <c r="O106">
         <v>5</v>
       </c>
-      <c r="M106">
-        <v>5</v>
-      </c>
-      <c r="N106">
-        <v>0</v>
-      </c>
-      <c r="O106">
-        <v>0</v>
-      </c>
       <c r="P106">
+        <v>2</v>
+      </c>
+      <c r="Q106">
+        <v>0</v>
+      </c>
+      <c r="R106">
         <v>1</v>
-      </c>
-      <c r="Q106">
-        <v>5</v>
-      </c>
-      <c r="R106">
-        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:18">
       <c r="A107">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B107">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D107" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E107">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F107">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G107">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H107">
+        <v>3</v>
+      </c>
+      <c r="I107">
         <v>4</v>
       </c>
-      <c r="I107">
-        <v>0</v>
-      </c>
       <c r="J107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K107">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L107">
         <v>2</v>
       </c>
       <c r="M107">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N107">
         <v>0</v>
       </c>
       <c r="O107">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P107">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q107">
         <v>0</v>
       </c>
       <c r="R107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:18">
       <c r="A108">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B108">
+        <v>15</v>
+      </c>
+      <c r="C108" t="s">
+        <v>124</v>
+      </c>
+      <c r="D108" t="s">
+        <v>139</v>
+      </c>
+      <c r="E108">
+        <v>7</v>
+      </c>
+      <c r="F108">
+        <v>7</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
+      <c r="H108">
+        <v>4</v>
+      </c>
+      <c r="I108">
         <v>2</v>
       </c>
-      <c r="C108" t="s">
-        <v>123</v>
-      </c>
-      <c r="D108" t="s">
-        <v>131</v>
-      </c>
-      <c r="E108">
-        <v>10</v>
-      </c>
-      <c r="F108">
-        <v>10</v>
-      </c>
-      <c r="G108">
-        <v>3</v>
-      </c>
-      <c r="H108">
-        <v>3</v>
-      </c>
-      <c r="I108">
+      <c r="J108">
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <v>1</v>
+      </c>
+      <c r="L108">
         <v>4</v>
       </c>
-      <c r="J108">
-        <v>0</v>
-      </c>
-      <c r="K108">
-        <v>3</v>
-      </c>
-      <c r="L108">
+      <c r="M108">
+        <v>0</v>
+      </c>
+      <c r="N108">
+        <v>0</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
+      </c>
+      <c r="P108">
+        <v>0</v>
+      </c>
+      <c r="Q108">
         <v>2</v>
-      </c>
-      <c r="M108">
-        <v>4</v>
-      </c>
-      <c r="N108">
-        <v>0</v>
-      </c>
-      <c r="O108">
-        <v>0</v>
-      </c>
-      <c r="P108">
-        <v>1</v>
-      </c>
-      <c r="Q108">
-        <v>0</v>
       </c>
       <c r="R108">
         <v>0</v>
@@ -6871,78 +6871,78 @@
     </row>
     <row r="109" spans="1:18">
       <c r="A109">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B109">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C109" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D109" t="s">
         <v>139</v>
       </c>
       <c r="E109">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F109">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H109">
+        <v>2</v>
+      </c>
+      <c r="I109">
         <v>4</v>
       </c>
-      <c r="I109">
+      <c r="J109">
+        <v>8</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>0</v>
+      </c>
+      <c r="M109">
+        <v>0</v>
+      </c>
+      <c r="N109">
+        <v>3</v>
+      </c>
+      <c r="O109">
+        <v>0</v>
+      </c>
+      <c r="P109">
         <v>2</v>
       </c>
-      <c r="J109">
-        <v>0</v>
-      </c>
-      <c r="K109">
-        <v>1</v>
-      </c>
-      <c r="L109">
+      <c r="Q109">
         <v>4</v>
       </c>
-      <c r="M109">
-        <v>0</v>
-      </c>
-      <c r="N109">
-        <v>0</v>
-      </c>
-      <c r="O109">
-        <v>0</v>
-      </c>
-      <c r="P109">
-        <v>0</v>
-      </c>
-      <c r="Q109">
-        <v>2</v>
-      </c>
       <c r="R109">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:18">
       <c r="A110">
+        <v>110</v>
+      </c>
+      <c r="B110">
         <v>109</v>
       </c>
-      <c r="B110">
-        <v>16</v>
-      </c>
       <c r="C110" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D110" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E110">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F110">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -6951,10 +6951,10 @@
         <v>2</v>
       </c>
       <c r="I110">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J110">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K110">
         <v>0</v>
@@ -6963,10 +6963,10 @@
         <v>0</v>
       </c>
       <c r="M110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N110">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O110">
         <v>0</v>
@@ -6975,7 +6975,7 @@
         <v>2</v>
       </c>
       <c r="Q110">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R110">
         <v>5</v>
@@ -6983,102 +6983,102 @@
     </row>
     <row r="111" spans="1:18">
       <c r="A111">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B111">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C111" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D111" t="s">
         <v>147</v>
       </c>
       <c r="E111">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F111">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G111">
         <v>0</v>
       </c>
       <c r="H111">
+        <v>1</v>
+      </c>
+      <c r="I111">
         <v>2</v>
       </c>
-      <c r="I111">
-        <v>3</v>
-      </c>
       <c r="J111">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K111">
         <v>0</v>
       </c>
       <c r="L111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M111">
+        <v>2</v>
+      </c>
+      <c r="N111">
         <v>1</v>
       </c>
-      <c r="N111">
-        <v>2</v>
-      </c>
       <c r="O111">
         <v>0</v>
       </c>
       <c r="P111">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q111">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R111">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:18">
       <c r="A112">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B112">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="C112" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D112" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E112">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F112">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G112">
         <v>0</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K112">
         <v>0</v>
       </c>
       <c r="L112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O112">
         <v>0</v>
@@ -7095,16 +7095,16 @@
     </row>
     <row r="113" spans="1:18">
       <c r="A113">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B113">
-        <v>88</v>
+        <v>3</v>
       </c>
       <c r="C113" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D113" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="E113">
         <v>0</v>
@@ -7146,118 +7146,6 @@
         <v>0</v>
       </c>
       <c r="R113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:18">
-      <c r="A114">
-        <v>113</v>
-      </c>
-      <c r="B114">
-        <v>3</v>
-      </c>
-      <c r="C114" t="s">
-        <v>129</v>
-      </c>
-      <c r="D114" t="s">
-        <v>131</v>
-      </c>
-      <c r="E114">
-        <v>0</v>
-      </c>
-      <c r="F114">
-        <v>0</v>
-      </c>
-      <c r="G114">
-        <v>0</v>
-      </c>
-      <c r="H114">
-        <v>0</v>
-      </c>
-      <c r="I114">
-        <v>0</v>
-      </c>
-      <c r="J114">
-        <v>0</v>
-      </c>
-      <c r="K114">
-        <v>0</v>
-      </c>
-      <c r="L114">
-        <v>0</v>
-      </c>
-      <c r="M114">
-        <v>0</v>
-      </c>
-      <c r="N114">
-        <v>0</v>
-      </c>
-      <c r="O114">
-        <v>0</v>
-      </c>
-      <c r="P114">
-        <v>0</v>
-      </c>
-      <c r="Q114">
-        <v>0</v>
-      </c>
-      <c r="R114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:18">
-      <c r="A115">
-        <v>114</v>
-      </c>
-      <c r="B115">
-        <v>60</v>
-      </c>
-      <c r="C115" t="s">
-        <v>104</v>
-      </c>
-      <c r="D115" t="s">
-        <v>134</v>
-      </c>
-      <c r="E115">
-        <v>0</v>
-      </c>
-      <c r="F115">
-        <v>0</v>
-      </c>
-      <c r="G115">
-        <v>0</v>
-      </c>
-      <c r="H115">
-        <v>0</v>
-      </c>
-      <c r="I115">
-        <v>0</v>
-      </c>
-      <c r="J115">
-        <v>0</v>
-      </c>
-      <c r="K115">
-        <v>0</v>
-      </c>
-      <c r="L115">
-        <v>0</v>
-      </c>
-      <c r="M115">
-        <v>0</v>
-      </c>
-      <c r="N115">
-        <v>0</v>
-      </c>
-      <c r="O115">
-        <v>0</v>
-      </c>
-      <c r="P115">
-        <v>0</v>
-      </c>
-      <c r="Q115">
-        <v>0</v>
-      </c>
-      <c r="R115">
         <v>0</v>
       </c>
     </row>

</xml_diff>